<commit_message>
Add sample of Item_DataMapper.kt to have an overview over how the mapper might look
</commit_message>
<xml_diff>
--- a/data/products.xlsx
+++ b/data/products.xlsx
@@ -28,7 +28,7 @@
     <t xml:space="preserve">name</t>
   </si>
   <si>
-    <t xml:space="preserve">quantity</t>
+    <t xml:space="preserve">available</t>
   </si>
   <si>
     <t xml:space="preserve">Bread</t>
@@ -65,8 +65,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
   <fonts count="7">
     <font>
@@ -156,7 +157,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -177,11 +178,19 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -206,17 +215,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F6" activeCellId="0" sqref="F6"/>
+      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.71484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="9.13"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -230,116 +239,117 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" s="5" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" s="6" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="n">
         <v>1000</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="4" t="n">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="3" s="7" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="6" t="n">
+      <c r="C2" s="5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" s="9" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="7" t="n">
         <v>1001</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="6" t="n">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="4" s="7" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="6" t="n">
+      <c r="C3" s="8" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" s="9" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="7" t="n">
         <v>1002</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="6" t="n">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" s="7" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="6" t="n">
+      <c r="C4" s="8" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" s="9" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="7" t="n">
         <v>1003</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="6" t="n">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="6" s="7" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="6" t="n">
+      <c r="C5" s="8" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" s="9" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="7" t="n">
         <v>1004</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="6" t="n">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="7" s="7" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="6" t="n">
+      <c r="C6" s="8" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" s="9" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="7" t="n">
         <v>1005</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="6" t="n">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="8" s="7" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="6" t="n">
+      <c r="C7" s="8" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" s="9" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="7" t="n">
         <v>1006</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="6" t="n">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="9" s="7" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="6" t="n">
+      <c r="C8" s="8" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" s="9" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="7" t="n">
         <v>1007</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="6" t="n">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="10" s="7" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="6" t="n">
+      <c r="C9" s="8" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" s="9" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="7" t="n">
         <v>1008</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="6" t="n">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="11" s="7" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="6" t="n">
+      <c r="C10" s="8" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" s="9" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="7" t="n">
         <v>1009</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="6" t="n">
-        <v>10</v>
-      </c>
-    </row>
+      <c r="C11" s="8" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>